<commit_message>
create classes for product and its components
</commit_message>
<xml_diff>
--- a/ExcelFiles/TaskLists/gtProductAssembly010819.xlsx
+++ b/ExcelFiles/TaskLists/gtProductAssembly010819.xlsx
@@ -1186,13 +1186,13 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1286,10 +1286,10 @@
     <tableColumn id="9" name="Total Minutes">
       <calculatedColumnFormula>+D2*B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Total Hours" dataDxfId="1">
+    <tableColumn id="10" name="Total Hours" dataDxfId="2">
       <calculatedColumnFormula>+E2/60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Cumulative Hours" dataDxfId="0">
+    <tableColumn id="11" name="Cumulative Hours" dataDxfId="1">
       <calculatedColumnFormula>SUM(F$2:F2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1306,7 +1306,7 @@
   <tableColumns count="3">
     <tableColumn id="12" name="Product"/>
     <tableColumn id="2" name="Part"/>
-    <tableColumn id="3" name="Quantity" dataDxfId="2"/>
+    <tableColumn id="3" name="Quantity" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1565,7 +1565,7 @@
   <dimension ref="A1:G116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -4535,8 +4535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C142"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="12" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
basis of all excel read task behavior
</commit_message>
<xml_diff>
--- a/ExcelFiles/TaskLists/gtProductAssembly010819.xlsx
+++ b/ExcelFiles/TaskLists/gtProductAssembly010819.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8540" yWindow="420" windowWidth="17520" windowHeight="15520" activeTab="1"/>
+    <workbookView xWindow="10860" yWindow="300" windowWidth="17520" windowHeight="15520"/>
   </bookViews>
   <sheets>
     <sheet name="tasks" sheetId="8" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="152">
   <si>
     <t>Product</t>
   </si>
@@ -170,9 +170,6 @@
   </si>
   <si>
     <t>Orange Sport Vest Set</t>
-  </si>
-  <si>
-    <t>BoosterSet</t>
   </si>
   <si>
     <t>PACK_FLEX_SML</t>
@@ -1564,8 +1561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1581,7 +1578,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1590,16 +1587,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" t="s">
         <v>149</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>150</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>151</v>
-      </c>
-      <c r="G1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2228,7 +2225,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B26">
         <v>33</v>
@@ -2306,7 +2303,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B29">
         <v>15</v>
@@ -2358,7 +2355,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="B31">
         <v>60</v>
@@ -2592,7 +2589,7 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B40">
         <v>60</v>
@@ -2745,7 +2742,7 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="B46">
         <v>60</v>
@@ -2823,7 +2820,7 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B49">
         <v>10</v>
@@ -3057,7 +3054,7 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B58">
         <v>11</v>
@@ -3083,7 +3080,7 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B59">
         <v>24</v>
@@ -3187,7 +3184,7 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B63">
         <v>60</v>
@@ -3213,7 +3210,7 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B64">
         <v>10</v>
@@ -3239,7 +3236,7 @@
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B65">
         <v>10</v>
@@ -3265,7 +3262,7 @@
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B66">
         <v>30</v>
@@ -3291,7 +3288,7 @@
     </row>
     <row r="67" spans="1:7">
       <c r="A67" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B67">
         <v>30</v>
@@ -3317,7 +3314,7 @@
     </row>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B68">
         <v>10</v>
@@ -3343,7 +3340,7 @@
     </row>
     <row r="69" spans="1:7">
       <c r="A69" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B69">
         <v>5</v>
@@ -3418,7 +3415,7 @@
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="B72">
         <v>60</v>
@@ -3626,7 +3623,7 @@
     </row>
     <row r="80" spans="1:7">
       <c r="A80" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B80">
         <v>10</v>
@@ -3652,7 +3649,7 @@
     </row>
     <row r="81" spans="1:7">
       <c r="A81" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B81">
         <v>10</v>
@@ -3678,7 +3675,7 @@
     </row>
     <row r="82" spans="1:7">
       <c r="A82" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B82">
         <v>10</v>
@@ -3704,7 +3701,7 @@
     </row>
     <row r="83" spans="1:7">
       <c r="A83" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B83">
         <v>40</v>
@@ -3730,7 +3727,7 @@
     </row>
     <row r="84" spans="1:7">
       <c r="A84" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B84">
         <v>20</v>
@@ -3756,7 +3753,7 @@
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B85">
         <v>20</v>
@@ -3782,7 +3779,7 @@
     </row>
     <row r="86" spans="1:7">
       <c r="A86" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B86">
         <v>40</v>
@@ -3808,7 +3805,7 @@
     </row>
     <row r="87" spans="1:7">
       <c r="A87" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B87">
         <v>40</v>
@@ -3834,7 +3831,7 @@
     </row>
     <row r="88" spans="1:7">
       <c r="A88" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B88">
         <v>20</v>
@@ -3860,7 +3857,7 @@
     </row>
     <row r="89" spans="1:7">
       <c r="A89" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B89">
         <v>20</v>
@@ -3886,7 +3883,7 @@
     </row>
     <row r="90" spans="1:7">
       <c r="A90" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B90">
         <v>20</v>
@@ -3912,7 +3909,7 @@
     </row>
     <row r="91" spans="1:7">
       <c r="A91" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B91">
         <v>20</v>
@@ -3938,7 +3935,7 @@
     </row>
     <row r="92" spans="1:7">
       <c r="A92" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B92">
         <v>10</v>
@@ -3964,7 +3961,7 @@
     </row>
     <row r="93" spans="1:7">
       <c r="A93" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B93">
         <v>10</v>
@@ -3990,7 +3987,7 @@
     </row>
     <row r="94" spans="1:7">
       <c r="A94" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B94">
         <v>10</v>
@@ -4016,7 +4013,7 @@
     </row>
     <row r="95" spans="1:7">
       <c r="A95" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B95">
         <v>10</v>
@@ -4042,7 +4039,7 @@
     </row>
     <row r="96" spans="1:7">
       <c r="A96" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B96">
         <v>10</v>
@@ -4068,7 +4065,7 @@
     </row>
     <row r="97" spans="1:7">
       <c r="A97" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B97">
         <v>10</v>
@@ -4094,7 +4091,7 @@
     </row>
     <row r="98" spans="1:7">
       <c r="A98" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B98">
         <v>20</v>
@@ -4518,6 +4515,11 @@
       <c r="F116" s="4"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A113">
+      <formula1>Products</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <tableParts count="1">
@@ -4535,8 +4537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -4551,15 +4553,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
@@ -4570,10 +4572,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -4595,7 +4597,7 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -4603,7 +4605,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -4614,10 +4616,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
@@ -4625,10 +4627,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
         <v>49</v>
-      </c>
-      <c r="B8" t="s">
-        <v>50</v>
       </c>
       <c r="C8" s="2">
         <v>4</v>
@@ -4636,10 +4638,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
         <v>54</v>
-      </c>
-      <c r="B9" t="s">
-        <v>55</v>
       </c>
       <c r="C9" s="2">
         <v>2</v>
@@ -4647,10 +4649,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
         <v>52</v>
-      </c>
-      <c r="B10" t="s">
-        <v>53</v>
       </c>
       <c r="C10" s="2">
         <v>4</v>
@@ -4658,10 +4660,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="2">
         <v>4</v>
@@ -4669,10 +4671,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="2">
         <v>4</v>
@@ -4680,7 +4682,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B13" t="s">
         <v>15</v>
@@ -4691,10 +4693,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C14" s="2">
         <v>1</v>
@@ -4702,7 +4704,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
@@ -4713,10 +4715,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C16" s="2">
         <v>1</v>
@@ -4724,10 +4726,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" s="2">
         <v>12</v>
@@ -4735,10 +4737,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C18" s="2">
         <v>1</v>
@@ -4746,7 +4748,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
         <v>15</v>
@@ -4757,10 +4759,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C20" s="2">
         <v>1</v>
@@ -4771,7 +4773,7 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C21" s="2">
         <v>4</v>
@@ -4782,7 +4784,7 @@
         <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C22" s="2">
         <v>4</v>
@@ -4793,7 +4795,7 @@
         <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C23" s="2">
         <v>1</v>
@@ -4804,7 +4806,7 @@
         <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C24" s="2">
         <v>4</v>
@@ -4815,7 +4817,7 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C25" s="2">
         <v>4</v>
@@ -4826,7 +4828,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C26" s="2">
         <v>1</v>
@@ -4837,7 +4839,7 @@
         <v>42</v>
       </c>
       <c r="B27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C27" s="2">
         <v>4</v>
@@ -4848,7 +4850,7 @@
         <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C28" s="2">
         <v>4</v>
@@ -4859,7 +4861,7 @@
         <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C29" s="2">
         <v>1</v>
@@ -4867,10 +4869,10 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C30" s="2">
         <v>4</v>
@@ -4878,10 +4880,10 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B31" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C31" s="2">
         <v>4</v>
@@ -4889,10 +4891,10 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C32" s="2">
         <v>1</v>
@@ -4911,7 +4913,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B34" t="s">
         <v>15</v>
@@ -4922,10 +4924,10 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C35" s="2">
         <v>1</v>
@@ -4936,7 +4938,7 @@
         <v>20</v>
       </c>
       <c r="B36" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C36" s="2">
         <v>4</v>
@@ -4947,7 +4949,7 @@
         <v>20</v>
       </c>
       <c r="B37" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C37" s="2">
         <v>4</v>
@@ -4958,7 +4960,7 @@
         <v>20</v>
       </c>
       <c r="B38" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C38" s="2">
         <v>1</v>
@@ -4966,10 +4968,10 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B39" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C39" s="2">
         <v>4</v>
@@ -4977,10 +4979,10 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B40" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C40" s="2">
         <v>4</v>
@@ -4988,10 +4990,10 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C41" s="2">
         <v>1</v>
@@ -4999,7 +5001,7 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B42" t="s">
         <v>15</v>
@@ -5010,10 +5012,10 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C43" s="2">
         <v>1</v>
@@ -5021,7 +5023,7 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B44" t="s">
         <v>15</v>
@@ -5032,10 +5034,10 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C45" s="2">
         <v>1</v>
@@ -5043,10 +5045,10 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C46" s="2">
         <v>12</v>
@@ -5054,10 +5056,10 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C47" s="2">
         <v>1</v>
@@ -5068,7 +5070,7 @@
         <v>43</v>
       </c>
       <c r="B48" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C48" s="2">
         <v>4</v>
@@ -5079,7 +5081,7 @@
         <v>43</v>
       </c>
       <c r="B49" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C49" s="2">
         <v>4</v>
@@ -5090,7 +5092,7 @@
         <v>43</v>
       </c>
       <c r="B50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C50" s="2">
         <v>1</v>
@@ -5098,7 +5100,7 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B51" t="s">
         <v>15</v>
@@ -5109,10 +5111,10 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B52" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C52" s="2">
         <v>1</v>
@@ -5123,7 +5125,7 @@
         <v>19</v>
       </c>
       <c r="B53" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C53" s="2">
         <v>4</v>
@@ -5134,7 +5136,7 @@
         <v>19</v>
       </c>
       <c r="B54" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C54" s="2">
         <v>4</v>
@@ -5145,7 +5147,7 @@
         <v>19</v>
       </c>
       <c r="B55" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C55" s="2">
         <v>1</v>
@@ -5156,7 +5158,7 @@
         <v>45</v>
       </c>
       <c r="B56" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C56" s="2">
         <v>4</v>
@@ -5167,7 +5169,7 @@
         <v>45</v>
       </c>
       <c r="B57" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C57" s="2">
         <v>4</v>
@@ -5178,7 +5180,7 @@
         <v>45</v>
       </c>
       <c r="B58" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C58" s="2">
         <v>1</v>
@@ -5186,7 +5188,7 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B59" t="s">
         <v>15</v>
@@ -5197,10 +5199,10 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B60" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C60" s="2">
         <v>1</v>
@@ -5222,7 +5224,7 @@
         <v>24</v>
       </c>
       <c r="B62" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C62" s="2">
         <v>1</v>
@@ -5230,7 +5232,7 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B63" t="s">
         <v>15</v>
@@ -5241,10 +5243,10 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B64" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C64" s="2">
         <v>1</v>
@@ -5252,7 +5254,7 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B65" t="s">
         <v>15</v>
@@ -5263,10 +5265,10 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B66" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C66" s="2">
         <v>1</v>
@@ -5277,7 +5279,7 @@
         <v>37</v>
       </c>
       <c r="B67" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C67" s="2">
         <v>4</v>
@@ -5288,7 +5290,7 @@
         <v>37</v>
       </c>
       <c r="B68" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C68" s="2">
         <v>4</v>
@@ -5299,7 +5301,7 @@
         <v>37</v>
       </c>
       <c r="B69" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C69" s="2">
         <v>1</v>
@@ -5307,7 +5309,7 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B70" t="s">
         <v>15</v>
@@ -5318,10 +5320,10 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C71" s="2">
         <v>1</v>
@@ -5343,7 +5345,7 @@
         <v>30</v>
       </c>
       <c r="B73" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C73" s="2">
         <v>1</v>
@@ -5365,7 +5367,7 @@
         <v>31</v>
       </c>
       <c r="B75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C75" s="2">
         <v>1</v>
@@ -5387,7 +5389,7 @@
         <v>32</v>
       </c>
       <c r="B77" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C77" s="2">
         <v>1</v>
@@ -5409,7 +5411,7 @@
         <v>33</v>
       </c>
       <c r="B79" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C79" s="2">
         <v>1</v>
@@ -5431,7 +5433,7 @@
         <v>34</v>
       </c>
       <c r="B81" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C81" s="2">
         <v>1</v>
@@ -5453,7 +5455,7 @@
         <v>35</v>
       </c>
       <c r="B83" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C83" s="2">
         <v>1</v>
@@ -5475,7 +5477,7 @@
         <v>36</v>
       </c>
       <c r="B85" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C85" s="2">
         <v>1</v>
@@ -5497,7 +5499,7 @@
         <v>38</v>
       </c>
       <c r="B87" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C87" s="2">
         <v>4</v>
@@ -5508,7 +5510,7 @@
         <v>38</v>
       </c>
       <c r="B88" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C88" s="2">
         <v>4</v>
@@ -5519,7 +5521,7 @@
         <v>38</v>
       </c>
       <c r="B89" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C89" s="2">
         <v>1</v>
@@ -5541,7 +5543,7 @@
         <v>25</v>
       </c>
       <c r="B91" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C91" s="2">
         <v>1</v>
@@ -5552,7 +5554,7 @@
         <v>27</v>
       </c>
       <c r="B92" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C92" s="2">
         <v>4</v>
@@ -5563,7 +5565,7 @@
         <v>27</v>
       </c>
       <c r="B93" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C93" s="2">
         <v>4</v>
@@ -5574,7 +5576,7 @@
         <v>27</v>
       </c>
       <c r="B94" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C94" s="2">
         <v>1</v>
@@ -5585,7 +5587,7 @@
         <v>46</v>
       </c>
       <c r="B95" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C95" s="2">
         <v>4</v>
@@ -5596,7 +5598,7 @@
         <v>46</v>
       </c>
       <c r="B96" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C96" s="2">
         <v>4</v>
@@ -5607,7 +5609,7 @@
         <v>46</v>
       </c>
       <c r="B97" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C97" s="2">
         <v>1</v>
@@ -5618,7 +5620,7 @@
         <v>39</v>
       </c>
       <c r="B98" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C98" s="2">
         <v>4</v>
@@ -5629,7 +5631,7 @@
         <v>39</v>
       </c>
       <c r="B99" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C99" s="2">
         <v>4</v>
@@ -5640,7 +5642,7 @@
         <v>39</v>
       </c>
       <c r="B100" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C100" s="2">
         <v>1</v>
@@ -5651,7 +5653,7 @@
         <v>40</v>
       </c>
       <c r="B101" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C101" s="2">
         <v>4</v>
@@ -5662,7 +5664,7 @@
         <v>40</v>
       </c>
       <c r="B102" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C102" s="2">
         <v>4</v>
@@ -5673,7 +5675,7 @@
         <v>40</v>
       </c>
       <c r="B103" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C103" s="2">
         <v>1</v>
@@ -5684,7 +5686,7 @@
         <v>44</v>
       </c>
       <c r="B104" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C104" s="2">
         <v>4</v>
@@ -5695,7 +5697,7 @@
         <v>44</v>
       </c>
       <c r="B105" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C105" s="2">
         <v>4</v>
@@ -5706,7 +5708,7 @@
         <v>44</v>
       </c>
       <c r="B106" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C106" s="2">
         <v>1</v>
@@ -5714,10 +5716,10 @@
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B107" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C107" s="2">
         <v>4</v>
@@ -5725,10 +5727,10 @@
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B108" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C108" s="2">
         <v>4</v>
@@ -5736,10 +5738,10 @@
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B109" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C109" s="2">
         <v>1</v>
@@ -5750,7 +5752,7 @@
         <v>21</v>
       </c>
       <c r="B110" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C110" s="2">
         <v>4</v>
@@ -5761,7 +5763,7 @@
         <v>21</v>
       </c>
       <c r="B111" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C111" s="2">
         <v>4</v>
@@ -5772,7 +5774,7 @@
         <v>21</v>
       </c>
       <c r="B112" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C112" s="2">
         <v>1</v>
@@ -5794,7 +5796,7 @@
         <v>23</v>
       </c>
       <c r="B114" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C114" s="2">
         <v>1</v>
@@ -5805,7 +5807,7 @@
         <v>41</v>
       </c>
       <c r="B115" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C115" s="2">
         <v>4</v>
@@ -5816,7 +5818,7 @@
         <v>41</v>
       </c>
       <c r="B116" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C116" s="2">
         <v>4</v>
@@ -5827,7 +5829,7 @@
         <v>41</v>
       </c>
       <c r="B117" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C117" s="2">
         <v>1</v>
@@ -5838,7 +5840,7 @@
         <v>28</v>
       </c>
       <c r="B118" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C118" s="2">
         <v>4</v>
@@ -5849,7 +5851,7 @@
         <v>28</v>
       </c>
       <c r="B119" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C119" s="2">
         <v>4</v>
@@ -5860,7 +5862,7 @@
         <v>28</v>
       </c>
       <c r="B120" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C120" s="2">
         <v>1</v>
@@ -5882,7 +5884,7 @@
         <v>29</v>
       </c>
       <c r="B122" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C122" s="2">
         <v>10</v>
@@ -5890,10 +5892,10 @@
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
+        <v>58</v>
+      </c>
+      <c r="B123" t="s">
         <v>59</v>
-      </c>
-      <c r="B123" t="s">
-        <v>60</v>
       </c>
       <c r="C123" s="2">
         <v>4</v>
@@ -5901,10 +5903,10 @@
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
+        <v>56</v>
+      </c>
+      <c r="B124" t="s">
         <v>57</v>
-      </c>
-      <c r="B124" t="s">
-        <v>58</v>
       </c>
       <c r="C124" s="2">
         <v>4</v>
@@ -5912,10 +5914,10 @@
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B125" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C125" s="2">
         <v>4</v>
@@ -5923,10 +5925,10 @@
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B126" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C126" s="2">
         <v>4</v>
@@ -5934,7 +5936,7 @@
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B127" t="s">
         <v>15</v>
@@ -5945,10 +5947,10 @@
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B128" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C128" s="2">
         <v>1</v>
@@ -5956,7 +5958,7 @@
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B129" t="s">
         <v>15</v>
@@ -5967,10 +5969,10 @@
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B130" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C130" s="2">
         <v>1</v>
@@ -5978,10 +5980,10 @@
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B131" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C131" s="2">
         <v>12</v>
@@ -5989,10 +5991,10 @@
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B132" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C132" s="2">
         <v>1</v>
@@ -6000,7 +6002,7 @@
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B133" t="s">
         <v>15</v>
@@ -6011,10 +6013,10 @@
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B134" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C134" s="2">
         <v>1</v>
@@ -6066,10 +6068,10 @@
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B139" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C139" s="2">
         <v>12</v>
@@ -6091,7 +6093,7 @@
         <v>5</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C141" s="2">
         <v>4</v>
@@ -6102,7 +6104,7 @@
         <v>5</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C142" s="6">
         <v>4</v>
@@ -6137,8 +6139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A68"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A68"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -6153,7 +6155,7 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:1">
@@ -6163,47 +6165,47 @@
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:1">
@@ -6223,7 +6225,7 @@
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:1">
@@ -6233,7 +6235,7 @@
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:1">
@@ -6243,22 +6245,22 @@
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:1">
@@ -6268,7 +6270,7 @@
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:1">
@@ -6283,7 +6285,7 @@
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:1">
@@ -6293,12 +6295,12 @@
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:1">
@@ -6308,7 +6310,7 @@
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:1">
@@ -6388,7 +6390,7 @@
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="50" spans="1:1">
@@ -6418,37 +6420,37 @@
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="62" spans="1:1">
@@ -6473,7 +6475,7 @@
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="1:1">
@@ -6520,7 +6522,7 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P1" t="str">
         <f>IFERROR(MID(#REF!,#REF!,#REF!),"")</f>
@@ -6541,7 +6543,7 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B3"/>
       <c r="I3" s="4"/>
@@ -6553,7 +6555,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B4"/>
       <c r="I4" s="4"/>
@@ -6577,7 +6579,7 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B6"/>
       <c r="I6" s="4"/>
@@ -6601,7 +6603,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B8"/>
       <c r="I8" s="4"/>
@@ -6625,7 +6627,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B10"/>
       <c r="I10" s="4"/>
@@ -6649,7 +6651,7 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B12"/>
       <c r="I12" s="4"/>
@@ -6661,7 +6663,7 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13"/>
       <c r="I13" s="4"/>
@@ -6673,7 +6675,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B14"/>
       <c r="I14" s="4"/>
@@ -6697,7 +6699,7 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B16"/>
       <c r="I16" s="4"/>
@@ -6721,7 +6723,7 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B18"/>
       <c r="I18" s="4"/>
@@ -6733,7 +6735,7 @@
     </row>
     <row r="19" spans="1:16">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B19"/>
       <c r="I19" s="4"/>
@@ -6745,7 +6747,7 @@
     </row>
     <row r="20" spans="1:16">
       <c r="A20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B20"/>
       <c r="I20" s="4"/>
@@ -6757,7 +6759,7 @@
     </row>
     <row r="21" spans="1:16">
       <c r="A21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B21"/>
       <c r="I21" s="4"/>
@@ -6769,7 +6771,7 @@
     </row>
     <row r="22" spans="1:16">
       <c r="A22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B22"/>
       <c r="I22" s="4"/>
@@ -6781,7 +6783,7 @@
     </row>
     <row r="23" spans="1:16">
       <c r="A23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B23"/>
       <c r="I23" s="4"/>
@@ -6793,7 +6795,7 @@
     </row>
     <row r="24" spans="1:16">
       <c r="A24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B24"/>
       <c r="I24" s="4"/>
@@ -6805,7 +6807,7 @@
     </row>
     <row r="25" spans="1:16">
       <c r="A25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B25"/>
       <c r="I25" s="4"/>
@@ -6817,7 +6819,7 @@
     </row>
     <row r="26" spans="1:16">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B26"/>
       <c r="I26" s="4"/>
@@ -6829,7 +6831,7 @@
     </row>
     <row r="27" spans="1:16">
       <c r="A27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B27"/>
       <c r="I27" s="4"/>
@@ -6841,7 +6843,7 @@
     </row>
     <row r="28" spans="1:16">
       <c r="A28" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B28"/>
       <c r="I28" s="4"/>
@@ -6853,7 +6855,7 @@
     </row>
     <row r="29" spans="1:16">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B29"/>
       <c r="I29" s="4"/>
@@ -6865,7 +6867,7 @@
     </row>
     <row r="30" spans="1:16">
       <c r="A30" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B30"/>
       <c r="I30" s="4"/>
@@ -6877,7 +6879,7 @@
     </row>
     <row r="31" spans="1:16">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B31"/>
       <c r="I31" s="4"/>
@@ -6889,7 +6891,7 @@
     </row>
     <row r="32" spans="1:16">
       <c r="A32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B32"/>
       <c r="I32" s="4"/>
@@ -6901,7 +6903,7 @@
     </row>
     <row r="33" spans="1:16">
       <c r="A33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B33"/>
       <c r="I33" s="4"/>
@@ -6913,7 +6915,7 @@
     </row>
     <row r="34" spans="1:16">
       <c r="A34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B34"/>
       <c r="I34" s="4"/>
@@ -6925,7 +6927,7 @@
     </row>
     <row r="35" spans="1:16">
       <c r="A35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B35"/>
       <c r="I35" s="4"/>
@@ -6937,7 +6939,7 @@
     </row>
     <row r="36" spans="1:16">
       <c r="A36" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B36"/>
       <c r="I36" s="4"/>
@@ -6949,7 +6951,7 @@
     </row>
     <row r="37" spans="1:16">
       <c r="A37" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B37"/>
       <c r="I37" s="4"/>
@@ -6961,7 +6963,7 @@
     </row>
     <row r="38" spans="1:16">
       <c r="A38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B38"/>
       <c r="I38" s="4"/>
@@ -6973,7 +6975,7 @@
     </row>
     <row r="39" spans="1:16">
       <c r="A39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B39"/>
       <c r="I39" s="4"/>
@@ -6985,7 +6987,7 @@
     </row>
     <row r="40" spans="1:16">
       <c r="A40" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B40"/>
       <c r="I40" s="4"/>
@@ -6997,7 +6999,7 @@
     </row>
     <row r="41" spans="1:16">
       <c r="A41" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B41"/>
       <c r="I41" s="4"/>
@@ -7009,7 +7011,7 @@
     </row>
     <row r="42" spans="1:16">
       <c r="A42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B42"/>
       <c r="I42" s="4"/>
@@ -7021,7 +7023,7 @@
     </row>
     <row r="43" spans="1:16">
       <c r="A43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B43"/>
       <c r="I43" s="4"/>
@@ -7033,7 +7035,7 @@
     </row>
     <row r="44" spans="1:16">
       <c r="A44" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B44"/>
       <c r="I44" s="4"/>
@@ -7045,7 +7047,7 @@
     </row>
     <row r="45" spans="1:16">
       <c r="A45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B45"/>
       <c r="I45" s="4"/>
@@ -7057,7 +7059,7 @@
     </row>
     <row r="46" spans="1:16">
       <c r="A46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B46"/>
       <c r="I46" s="4"/>
@@ -7069,7 +7071,7 @@
     </row>
     <row r="47" spans="1:16">
       <c r="A47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B47"/>
       <c r="I47" s="4"/>
@@ -7081,7 +7083,7 @@
     </row>
     <row r="48" spans="1:16">
       <c r="A48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B48"/>
       <c r="I48" s="4"/>
@@ -7093,7 +7095,7 @@
     </row>
     <row r="49" spans="1:16">
       <c r="A49" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B49"/>
       <c r="I49" s="4"/>
@@ -7105,7 +7107,7 @@
     </row>
     <row r="50" spans="1:16">
       <c r="A50" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B50"/>
       <c r="I50" s="4"/>
@@ -7117,7 +7119,7 @@
     </row>
     <row r="51" spans="1:16">
       <c r="A51" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B51"/>
       <c r="I51" s="4"/>
@@ -7129,7 +7131,7 @@
     </row>
     <row r="52" spans="1:16">
       <c r="A52" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B52"/>
       <c r="I52" s="4"/>
@@ -7141,7 +7143,7 @@
     </row>
     <row r="53" spans="1:16">
       <c r="A53" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B53"/>
       <c r="I53" s="4"/>
@@ -7153,7 +7155,7 @@
     </row>
     <row r="54" spans="1:16">
       <c r="A54" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B54"/>
       <c r="I54" s="4"/>
@@ -7165,7 +7167,7 @@
     </row>
     <row r="55" spans="1:16">
       <c r="A55" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B55"/>
       <c r="I55" s="4"/>
@@ -7177,7 +7179,7 @@
     </row>
     <row r="56" spans="1:16">
       <c r="A56" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B56"/>
       <c r="I56" s="4"/>
@@ -7189,7 +7191,7 @@
     </row>
     <row r="57" spans="1:16">
       <c r="A57" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B57"/>
       <c r="I57" s="4"/>
@@ -7201,7 +7203,7 @@
     </row>
     <row r="58" spans="1:16">
       <c r="A58" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B58"/>
       <c r="I58" s="4"/>
@@ -7213,7 +7215,7 @@
     </row>
     <row r="59" spans="1:16">
       <c r="A59" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B59"/>
       <c r="I59" s="4"/>
@@ -7225,7 +7227,7 @@
     </row>
     <row r="60" spans="1:16">
       <c r="A60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B60"/>
       <c r="I60" s="4"/>
@@ -7237,7 +7239,7 @@
     </row>
     <row r="61" spans="1:16">
       <c r="A61" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B61"/>
       <c r="I61" s="4"/>
@@ -7249,7 +7251,7 @@
     </row>
     <row r="62" spans="1:16">
       <c r="A62" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B62"/>
       <c r="I62" s="4"/>
@@ -7261,7 +7263,7 @@
     </row>
     <row r="63" spans="1:16">
       <c r="A63" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B63"/>
       <c r="I63" s="4"/>
@@ -7273,7 +7275,7 @@
     </row>
     <row r="64" spans="1:16">
       <c r="A64" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B64"/>
       <c r="I64" s="4"/>
@@ -7285,7 +7287,7 @@
     </row>
     <row r="65" spans="1:16">
       <c r="A65" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B65"/>
       <c r="I65" s="4"/>
@@ -7297,7 +7299,7 @@
     </row>
     <row r="66" spans="1:16">
       <c r="A66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B66"/>
       <c r="I66" s="4"/>
@@ -7309,7 +7311,7 @@
     </row>
     <row r="67" spans="1:16">
       <c r="A67" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B67"/>
       <c r="I67" s="4"/>
@@ -7321,7 +7323,7 @@
     </row>
     <row r="68" spans="1:16">
       <c r="A68" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B68"/>
       <c r="I68" s="4"/>
@@ -7329,40 +7331,40 @@
     </row>
     <row r="69" spans="1:16">
       <c r="A69" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I69" s="4"/>
     </row>
     <row r="70" spans="1:16">
       <c r="A70" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I70" s="4"/>
     </row>
     <row r="71" spans="1:16">
       <c r="A71" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I71" s="4"/>
     </row>
     <row r="72" spans="1:16">
       <c r="A72" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="73" spans="1:16">
       <c r="A73" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="74" spans="1:16">
       <c r="A74" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="75" spans="1:16">
       <c r="A75" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="76" spans="1:16">

</xml_diff>